<commit_message>
Versionado de lecciones aprendidas
</commit_message>
<xml_diff>
--- a/Organización/IWM_LeccionesAprendidas.xlsx
+++ b/Organización/IWM_LeccionesAprendidas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\IWM\Repositorio IWM\Organización\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zepeda\Documents\cabina_press\Organización\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="53">
   <si>
     <t>LECCION APRENDIDA</t>
   </si>
@@ -176,6 +176,15 @@
   </si>
   <si>
     <t>Auditar los primero documentos generados, despues aprobarlos en direccion y finalmente por el cliente</t>
+  </si>
+  <si>
+    <t>Global</t>
+  </si>
+  <si>
+    <t>Capacitacion</t>
+  </si>
+  <si>
+    <t>Control en archivos de repositorio (versionado adecuado para evitar conflictos)</t>
   </si>
 </sst>
 </file>
@@ -294,14 +303,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -592,8 +601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,13 +615,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
@@ -873,16 +882,16 @@
       <c r="B18" s="3">
         <v>15</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="C18" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="9" t="s">
         <v>30</v>
       </c>
     </row>
@@ -890,10 +899,18 @@
       <c r="B19" s="3">
         <v>16</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
+      <c r="C19" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="3">

</xml_diff>